<commit_message>
Just for save ;)
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F186"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,16 +491,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -510,16 +510,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -529,16 +529,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7">
@@ -548,16 +548,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
@@ -567,16 +567,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
@@ -599,7 +599,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>(0, 2)</t>
+          <t>(0, 1)</t>
         </is>
       </c>
     </row>
@@ -648,13 +648,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -667,16 +667,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
@@ -686,16 +686,16 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
@@ -705,16 +705,16 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
@@ -737,7 +737,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>(1, 0)</t>
+          <t>(0, 2)</t>
         </is>
       </c>
     </row>
@@ -748,7 +748,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
@@ -757,7 +757,7 @@
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -767,7 +767,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
@@ -776,7 +776,7 @@
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -786,13 +786,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -805,13 +805,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
@@ -843,10 +843,10 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -875,7 +875,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>(1, 3)</t>
+          <t>(0, 3)</t>
         </is>
       </c>
     </row>
@@ -968,10 +968,10 @@
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1013,7 +1013,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>(3, 0)</t>
+          <t>(1, 0)</t>
         </is>
       </c>
     </row>
@@ -1049,10 +1049,10 @@
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1062,16 +1062,16 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38">
@@ -1081,16 +1081,16 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D38" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39">
@@ -1100,13 +1100,13 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E39" t="n">
         <v>0</v>
@@ -1119,16 +1119,16 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41">
@@ -1151,7 +1151,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>(3, 1)</t>
+          <t>(1, 1)</t>
         </is>
       </c>
     </row>
@@ -1200,16 +1200,16 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -1219,16 +1219,16 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C46" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47">
@@ -1238,16 +1238,16 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
@@ -1257,16 +1257,16 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -1284,41 +1284,38 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>AWAY</t>
+          <t>SCORE</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>TEAM</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>IS</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>FAVORITE</t>
+          <t>(1, 2)</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>SCORE</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>(0, 1)</t>
-        </is>
+          <t>ULTRA</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>0</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>ULTRA</t>
+          <t>SUPER</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1337,7 +1334,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>SUPER</t>
+          <t>HUGE</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1356,7 +1353,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>HUGE</t>
+          <t>STRONG</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1375,14 +1372,14 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>STRONG</t>
+          <t>LITE</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D55" t="n">
         <v>0</v>
@@ -1394,17 +1391,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>LITE</t>
+          <t>EQUAL</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E56" t="n">
         <v>0</v>
@@ -1413,29 +1410,2240 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>EQUAL</t>
-        </is>
-      </c>
-      <c r="B57" t="n">
-        <v>1</v>
-      </c>
-      <c r="C57" t="n">
-        <v>0</v>
-      </c>
-      <c r="D57" t="n">
-        <v>0</v>
-      </c>
-      <c r="E57" t="n">
-        <v>1</v>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t> </t>
+          <t>SCORE</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
+        <is>
+          <t>(2, 0)</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>ULTRA</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>0</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>SUPER</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>1</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>HUGE</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>4</v>
+      </c>
+      <c r="C61" t="n">
+        <v>3</v>
+      </c>
+      <c r="D61" t="n">
+        <v>1</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>STRONG</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>4</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0</v>
+      </c>
+      <c r="D62" t="n">
+        <v>3</v>
+      </c>
+      <c r="E62" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>LITE</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>1</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0</v>
+      </c>
+      <c r="D63" t="n">
+        <v>1</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>EQUAL</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>2</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0</v>
+      </c>
+      <c r="D64" t="n">
+        <v>1</v>
+      </c>
+      <c r="E64" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>SCORE</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>(2, 1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>ULTRA</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>0</v>
+      </c>
+      <c r="C67" t="n">
+        <v>0</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>SUPER</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>0</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>HUGE</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>0</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>STRONG</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>1</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0</v>
+      </c>
+      <c r="E70" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>LITE</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>2</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0</v>
+      </c>
+      <c r="D71" t="n">
+        <v>1</v>
+      </c>
+      <c r="E71" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>EQUAL</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>4</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0</v>
+      </c>
+      <c r="D72" t="n">
+        <v>3</v>
+      </c>
+      <c r="E72" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>SCORE</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>(2, 2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>ULTRA</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>0</v>
+      </c>
+      <c r="C75" t="n">
+        <v>0</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>SUPER</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>0</v>
+      </c>
+      <c r="C76" t="n">
+        <v>0</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>HUGE</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>0</v>
+      </c>
+      <c r="C77" t="n">
+        <v>0</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>STRONG</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>0</v>
+      </c>
+      <c r="C78" t="n">
+        <v>0</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>LITE</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>1</v>
+      </c>
+      <c r="C79" t="n">
+        <v>0</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E79" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>EQUAL</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>0</v>
+      </c>
+      <c r="C80" t="n">
+        <v>0</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>SCORE</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>(2, 4)</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>ULTRA</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>0</v>
+      </c>
+      <c r="C83" t="n">
+        <v>0</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>SUPER</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>0</v>
+      </c>
+      <c r="C84" t="n">
+        <v>0</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>HUGE</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>0</v>
+      </c>
+      <c r="C85" t="n">
+        <v>0</v>
+      </c>
+      <c r="D85" t="n">
+        <v>0</v>
+      </c>
+      <c r="E85" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>STRONG</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>0</v>
+      </c>
+      <c r="C86" t="n">
+        <v>0</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>LITE</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>0</v>
+      </c>
+      <c r="C87" t="n">
+        <v>0</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>EQUAL</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>1</v>
+      </c>
+      <c r="C88" t="n">
+        <v>0</v>
+      </c>
+      <c r="D88" t="n">
+        <v>1</v>
+      </c>
+      <c r="E88" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>SCORE</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>(3, 0)</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>ULTRA</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>0</v>
+      </c>
+      <c r="C91" t="n">
+        <v>0</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>SUPER</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>0</v>
+      </c>
+      <c r="C92" t="n">
+        <v>0</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>HUGE</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>2</v>
+      </c>
+      <c r="C93" t="n">
+        <v>1</v>
+      </c>
+      <c r="D93" t="n">
+        <v>1</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>STRONG</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>2</v>
+      </c>
+      <c r="C94" t="n">
+        <v>1</v>
+      </c>
+      <c r="D94" t="n">
+        <v>1</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>LITE</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>1</v>
+      </c>
+      <c r="C95" t="n">
+        <v>0</v>
+      </c>
+      <c r="D95" t="n">
+        <v>0</v>
+      </c>
+      <c r="E95" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>EQUAL</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>1</v>
+      </c>
+      <c r="C96" t="n">
+        <v>0</v>
+      </c>
+      <c r="D96" t="n">
+        <v>0</v>
+      </c>
+      <c r="E96" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>SCORE</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>(4, 0)</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>ULTRA</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>0</v>
+      </c>
+      <c r="C99" t="n">
+        <v>0</v>
+      </c>
+      <c r="D99" t="n">
+        <v>0</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>SUPER</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>0</v>
+      </c>
+      <c r="C100" t="n">
+        <v>0</v>
+      </c>
+      <c r="D100" t="n">
+        <v>0</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>HUGE</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>0</v>
+      </c>
+      <c r="C101" t="n">
+        <v>0</v>
+      </c>
+      <c r="D101" t="n">
+        <v>0</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>STRONG</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>1</v>
+      </c>
+      <c r="C102" t="n">
+        <v>1</v>
+      </c>
+      <c r="D102" t="n">
+        <v>0</v>
+      </c>
+      <c r="E102" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>LITE</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>0</v>
+      </c>
+      <c r="C103" t="n">
+        <v>0</v>
+      </c>
+      <c r="D103" t="n">
+        <v>0</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>EQUAL</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>0</v>
+      </c>
+      <c r="C104" t="n">
+        <v>0</v>
+      </c>
+      <c r="D104" t="n">
+        <v>0</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>SCORE</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>(4, 1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>ULTRA</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>0</v>
+      </c>
+      <c r="C107" t="n">
+        <v>0</v>
+      </c>
+      <c r="D107" t="n">
+        <v>0</v>
+      </c>
+      <c r="E107" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>SUPER</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>0</v>
+      </c>
+      <c r="C108" t="n">
+        <v>0</v>
+      </c>
+      <c r="D108" t="n">
+        <v>0</v>
+      </c>
+      <c r="E108" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>HUGE</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>1</v>
+      </c>
+      <c r="C109" t="n">
+        <v>0</v>
+      </c>
+      <c r="D109" t="n">
+        <v>0</v>
+      </c>
+      <c r="E109" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>STRONG</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>1</v>
+      </c>
+      <c r="C110" t="n">
+        <v>0</v>
+      </c>
+      <c r="D110" t="n">
+        <v>0</v>
+      </c>
+      <c r="E110" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>LITE</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>1</v>
+      </c>
+      <c r="C111" t="n">
+        <v>0</v>
+      </c>
+      <c r="D111" t="n">
+        <v>0</v>
+      </c>
+      <c r="E111" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>EQUAL</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>0</v>
+      </c>
+      <c r="C112" t="n">
+        <v>0</v>
+      </c>
+      <c r="D112" t="n">
+        <v>0</v>
+      </c>
+      <c r="E112" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>AWAY</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>TEAM</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>IS</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>FAVORITE</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>SCORE</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>(0, 0)</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>ULTRA</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>0</v>
+      </c>
+      <c r="C116" t="n">
+        <v>0</v>
+      </c>
+      <c r="D116" t="n">
+        <v>0</v>
+      </c>
+      <c r="E116" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>SUPER</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>0</v>
+      </c>
+      <c r="C117" t="n">
+        <v>0</v>
+      </c>
+      <c r="D117" t="n">
+        <v>0</v>
+      </c>
+      <c r="E117" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>HUGE</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>1</v>
+      </c>
+      <c r="C118" t="n">
+        <v>0</v>
+      </c>
+      <c r="D118" t="n">
+        <v>0</v>
+      </c>
+      <c r="E118" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>STRONG</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>3</v>
+      </c>
+      <c r="C119" t="n">
+        <v>0</v>
+      </c>
+      <c r="D119" t="n">
+        <v>0</v>
+      </c>
+      <c r="E119" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>LITE</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>7</v>
+      </c>
+      <c r="C120" t="n">
+        <v>1</v>
+      </c>
+      <c r="D120" t="n">
+        <v>3</v>
+      </c>
+      <c r="E120" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>EQUAL</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>6</v>
+      </c>
+      <c r="C121" t="n">
+        <v>2</v>
+      </c>
+      <c r="D121" t="n">
+        <v>2</v>
+      </c>
+      <c r="E121" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>SCORE</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>(0, 1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>ULTRA</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>0</v>
+      </c>
+      <c r="C124" t="n">
+        <v>0</v>
+      </c>
+      <c r="D124" t="n">
+        <v>0</v>
+      </c>
+      <c r="E124" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>SUPER</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>0</v>
+      </c>
+      <c r="C125" t="n">
+        <v>0</v>
+      </c>
+      <c r="D125" t="n">
+        <v>0</v>
+      </c>
+      <c r="E125" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>HUGE</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>1</v>
+      </c>
+      <c r="C126" t="n">
+        <v>0</v>
+      </c>
+      <c r="D126" t="n">
+        <v>0</v>
+      </c>
+      <c r="E126" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>STRONG</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>2</v>
+      </c>
+      <c r="C127" t="n">
+        <v>0</v>
+      </c>
+      <c r="D127" t="n">
+        <v>0</v>
+      </c>
+      <c r="E127" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>LITE</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>5</v>
+      </c>
+      <c r="C128" t="n">
+        <v>0</v>
+      </c>
+      <c r="D128" t="n">
+        <v>2</v>
+      </c>
+      <c r="E128" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>EQUAL</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>7</v>
+      </c>
+      <c r="C129" t="n">
+        <v>2</v>
+      </c>
+      <c r="D129" t="n">
+        <v>1</v>
+      </c>
+      <c r="E129" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>SCORE</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>(0, 2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>ULTRA</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>0</v>
+      </c>
+      <c r="C132" t="n">
+        <v>0</v>
+      </c>
+      <c r="D132" t="n">
+        <v>0</v>
+      </c>
+      <c r="E132" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>SUPER</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
+        <v>0</v>
+      </c>
+      <c r="C133" t="n">
+        <v>0</v>
+      </c>
+      <c r="D133" t="n">
+        <v>0</v>
+      </c>
+      <c r="E133" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>HUGE</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>0</v>
+      </c>
+      <c r="C134" t="n">
+        <v>0</v>
+      </c>
+      <c r="D134" t="n">
+        <v>0</v>
+      </c>
+      <c r="E134" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>STRONG</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
+        <v>2</v>
+      </c>
+      <c r="C135" t="n">
+        <v>1</v>
+      </c>
+      <c r="D135" t="n">
+        <v>0</v>
+      </c>
+      <c r="E135" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>LITE</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>2</v>
+      </c>
+      <c r="C136" t="n">
+        <v>0</v>
+      </c>
+      <c r="D136" t="n">
+        <v>1</v>
+      </c>
+      <c r="E136" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>EQUAL</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>1</v>
+      </c>
+      <c r="C137" t="n">
+        <v>0</v>
+      </c>
+      <c r="D137" t="n">
+        <v>0</v>
+      </c>
+      <c r="E137" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>SCORE</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>(1, 0)</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>ULTRA</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>0</v>
+      </c>
+      <c r="C140" t="n">
+        <v>0</v>
+      </c>
+      <c r="D140" t="n">
+        <v>0</v>
+      </c>
+      <c r="E140" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>SUPER</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>0</v>
+      </c>
+      <c r="C141" t="n">
+        <v>0</v>
+      </c>
+      <c r="D141" t="n">
+        <v>0</v>
+      </c>
+      <c r="E141" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>HUGE</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>0</v>
+      </c>
+      <c r="C142" t="n">
+        <v>0</v>
+      </c>
+      <c r="D142" t="n">
+        <v>0</v>
+      </c>
+      <c r="E142" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>STRONG</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
+        <v>0</v>
+      </c>
+      <c r="C143" t="n">
+        <v>0</v>
+      </c>
+      <c r="D143" t="n">
+        <v>0</v>
+      </c>
+      <c r="E143" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>LITE</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>7</v>
+      </c>
+      <c r="C144" t="n">
+        <v>2</v>
+      </c>
+      <c r="D144" t="n">
+        <v>3</v>
+      </c>
+      <c r="E144" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>EQUAL</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
+        <v>2</v>
+      </c>
+      <c r="C145" t="n">
+        <v>1</v>
+      </c>
+      <c r="D145" t="n">
+        <v>0</v>
+      </c>
+      <c r="E145" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>SCORE</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>(1, 1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>ULTRA</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
+        <v>0</v>
+      </c>
+      <c r="C148" t="n">
+        <v>0</v>
+      </c>
+      <c r="D148" t="n">
+        <v>0</v>
+      </c>
+      <c r="E148" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>SUPER</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
+        <v>0</v>
+      </c>
+      <c r="C149" t="n">
+        <v>0</v>
+      </c>
+      <c r="D149" t="n">
+        <v>0</v>
+      </c>
+      <c r="E149" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>HUGE</t>
+        </is>
+      </c>
+      <c r="B150" t="n">
+        <v>0</v>
+      </c>
+      <c r="C150" t="n">
+        <v>0</v>
+      </c>
+      <c r="D150" t="n">
+        <v>0</v>
+      </c>
+      <c r="E150" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>STRONG</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
+        <v>0</v>
+      </c>
+      <c r="C151" t="n">
+        <v>0</v>
+      </c>
+      <c r="D151" t="n">
+        <v>0</v>
+      </c>
+      <c r="E151" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>LITE</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>3</v>
+      </c>
+      <c r="C152" t="n">
+        <v>0</v>
+      </c>
+      <c r="D152" t="n">
+        <v>0</v>
+      </c>
+      <c r="E152" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>EQUAL</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>1</v>
+      </c>
+      <c r="C153" t="n">
+        <v>0</v>
+      </c>
+      <c r="D153" t="n">
+        <v>0</v>
+      </c>
+      <c r="E153" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>SCORE</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>(1, 2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>ULTRA</t>
+        </is>
+      </c>
+      <c r="B156" t="n">
+        <v>0</v>
+      </c>
+      <c r="C156" t="n">
+        <v>0</v>
+      </c>
+      <c r="D156" t="n">
+        <v>0</v>
+      </c>
+      <c r="E156" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>SUPER</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
+        <v>0</v>
+      </c>
+      <c r="C157" t="n">
+        <v>0</v>
+      </c>
+      <c r="D157" t="n">
+        <v>0</v>
+      </c>
+      <c r="E157" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>HUGE</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>0</v>
+      </c>
+      <c r="C158" t="n">
+        <v>0</v>
+      </c>
+      <c r="D158" t="n">
+        <v>0</v>
+      </c>
+      <c r="E158" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>STRONG</t>
+        </is>
+      </c>
+      <c r="B159" t="n">
+        <v>1</v>
+      </c>
+      <c r="C159" t="n">
+        <v>1</v>
+      </c>
+      <c r="D159" t="n">
+        <v>0</v>
+      </c>
+      <c r="E159" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>LITE</t>
+        </is>
+      </c>
+      <c r="B160" t="n">
+        <v>2</v>
+      </c>
+      <c r="C160" t="n">
+        <v>0</v>
+      </c>
+      <c r="D160" t="n">
+        <v>1</v>
+      </c>
+      <c r="E160" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>EQUAL</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
+        <v>0</v>
+      </c>
+      <c r="C161" t="n">
+        <v>0</v>
+      </c>
+      <c r="D161" t="n">
+        <v>0</v>
+      </c>
+      <c r="E161" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>SCORE</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>(2, 0)</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>ULTRA</t>
+        </is>
+      </c>
+      <c r="B164" t="n">
+        <v>0</v>
+      </c>
+      <c r="C164" t="n">
+        <v>0</v>
+      </c>
+      <c r="D164" t="n">
+        <v>0</v>
+      </c>
+      <c r="E164" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>SUPER</t>
+        </is>
+      </c>
+      <c r="B165" t="n">
+        <v>0</v>
+      </c>
+      <c r="C165" t="n">
+        <v>0</v>
+      </c>
+      <c r="D165" t="n">
+        <v>0</v>
+      </c>
+      <c r="E165" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>HUGE</t>
+        </is>
+      </c>
+      <c r="B166" t="n">
+        <v>0</v>
+      </c>
+      <c r="C166" t="n">
+        <v>0</v>
+      </c>
+      <c r="D166" t="n">
+        <v>0</v>
+      </c>
+      <c r="E166" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>STRONG</t>
+        </is>
+      </c>
+      <c r="B167" t="n">
+        <v>1</v>
+      </c>
+      <c r="C167" t="n">
+        <v>0</v>
+      </c>
+      <c r="D167" t="n">
+        <v>0</v>
+      </c>
+      <c r="E167" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>LITE</t>
+        </is>
+      </c>
+      <c r="B168" t="n">
+        <v>1</v>
+      </c>
+      <c r="C168" t="n">
+        <v>0</v>
+      </c>
+      <c r="D168" t="n">
+        <v>1</v>
+      </c>
+      <c r="E168" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>EQUAL</t>
+        </is>
+      </c>
+      <c r="B169" t="n">
+        <v>1</v>
+      </c>
+      <c r="C169" t="n">
+        <v>0</v>
+      </c>
+      <c r="D169" t="n">
+        <v>0</v>
+      </c>
+      <c r="E169" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>SCORE</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>(2, 1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>ULTRA</t>
+        </is>
+      </c>
+      <c r="B172" t="n">
+        <v>0</v>
+      </c>
+      <c r="C172" t="n">
+        <v>0</v>
+      </c>
+      <c r="D172" t="n">
+        <v>0</v>
+      </c>
+      <c r="E172" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>SUPER</t>
+        </is>
+      </c>
+      <c r="B173" t="n">
+        <v>0</v>
+      </c>
+      <c r="C173" t="n">
+        <v>0</v>
+      </c>
+      <c r="D173" t="n">
+        <v>0</v>
+      </c>
+      <c r="E173" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>HUGE</t>
+        </is>
+      </c>
+      <c r="B174" t="n">
+        <v>0</v>
+      </c>
+      <c r="C174" t="n">
+        <v>0</v>
+      </c>
+      <c r="D174" t="n">
+        <v>0</v>
+      </c>
+      <c r="E174" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>STRONG</t>
+        </is>
+      </c>
+      <c r="B175" t="n">
+        <v>1</v>
+      </c>
+      <c r="C175" t="n">
+        <v>0</v>
+      </c>
+      <c r="D175" t="n">
+        <v>0</v>
+      </c>
+      <c r="E175" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>LITE</t>
+        </is>
+      </c>
+      <c r="B176" t="n">
+        <v>0</v>
+      </c>
+      <c r="C176" t="n">
+        <v>0</v>
+      </c>
+      <c r="D176" t="n">
+        <v>0</v>
+      </c>
+      <c r="E176" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>EQUAL</t>
+        </is>
+      </c>
+      <c r="B177" t="n">
+        <v>1</v>
+      </c>
+      <c r="C177" t="n">
+        <v>0</v>
+      </c>
+      <c r="D177" t="n">
+        <v>1</v>
+      </c>
+      <c r="E177" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>SCORE</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>(2, 2)</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>ULTRA</t>
+        </is>
+      </c>
+      <c r="B180" t="n">
+        <v>0</v>
+      </c>
+      <c r="C180" t="n">
+        <v>0</v>
+      </c>
+      <c r="D180" t="n">
+        <v>0</v>
+      </c>
+      <c r="E180" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>SUPER</t>
+        </is>
+      </c>
+      <c r="B181" t="n">
+        <v>0</v>
+      </c>
+      <c r="C181" t="n">
+        <v>0</v>
+      </c>
+      <c r="D181" t="n">
+        <v>0</v>
+      </c>
+      <c r="E181" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>HUGE</t>
+        </is>
+      </c>
+      <c r="B182" t="n">
+        <v>0</v>
+      </c>
+      <c r="C182" t="n">
+        <v>0</v>
+      </c>
+      <c r="D182" t="n">
+        <v>0</v>
+      </c>
+      <c r="E182" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>STRONG</t>
+        </is>
+      </c>
+      <c r="B183" t="n">
+        <v>0</v>
+      </c>
+      <c r="C183" t="n">
+        <v>0</v>
+      </c>
+      <c r="D183" t="n">
+        <v>0</v>
+      </c>
+      <c r="E183" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>LITE</t>
+        </is>
+      </c>
+      <c r="B184" t="n">
+        <v>1</v>
+      </c>
+      <c r="C184" t="n">
+        <v>0</v>
+      </c>
+      <c r="D184" t="n">
+        <v>1</v>
+      </c>
+      <c r="E184" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>EQUAL</t>
+        </is>
+      </c>
+      <c r="B185" t="n">
+        <v>0</v>
+      </c>
+      <c r="C185" t="n">
+        <v>0</v>
+      </c>
+      <c r="D185" t="n">
+        <v>0</v>
+      </c>
+      <c r="E185" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
         <is>
           <t> </t>
         </is>

</xml_diff>